<commit_message>
Terminarios cap 1 terminados y avances con la presentacion
</commit_message>
<xml_diff>
--- a/src/Contenido_Encovi_Departamentales.xlsx
+++ b/src/Contenido_Encovi_Departamentales.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="183">
   <si>
     <t xml:space="preserve">Numero capítulo</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">Distribución población según idioma en que aprendió a hablar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">año 2014 </t>
   </si>
   <si>
     <t xml:space="preserve">Población que habla más de un idioma</t>
@@ -750,23 +753,23 @@
   </sheetPr>
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="D38" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
-      <selection pane="topRight" activeCell="J49" activeCellId="0" sqref="J49"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.1071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="75.3265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="63.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.5663265306123"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="74.3826530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="62.9081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,7 +1119,7 @@
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>23</v>
@@ -1130,10 +1133,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>17</v>
@@ -1156,10 +1159,10 @@
         <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>17</v>
@@ -1174,7 +1177,7 @@
         <v>23</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,10 +1188,10 @@
         <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>17</v>
@@ -1211,10 +1214,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>17</v>
@@ -1229,7 +1232,7 @@
         <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1240,10 +1243,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>17</v>
@@ -1258,7 +1261,7 @@
         <v>23</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,10 +1272,10 @@
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>17</v>
@@ -1295,10 +1298,10 @@
         <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>17</v>
@@ -1321,10 +1324,10 @@
         <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>17</v>
@@ -1347,10 +1350,10 @@
         <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>17</v>
@@ -1373,10 +1376,10 @@
         <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>17</v>
@@ -1399,10 +1402,10 @@
         <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>17</v>
@@ -1422,13 +1425,13 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -1451,13 +1454,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
@@ -1477,13 +1480,13 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
@@ -1506,13 +1509,13 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1532,13 +1535,13 @@
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1561,13 +1564,13 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1587,13 +1590,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
@@ -1613,13 +1616,13 @@
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1639,13 +1642,13 @@
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1665,13 +1668,13 @@
         <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1691,13 +1694,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1717,13 +1720,13 @@
         <v>2</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1743,13 +1746,13 @@
         <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1758,7 +1761,7 @@
         <v>14</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>23</v>
@@ -1769,13 +1772,13 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1798,13 +1801,13 @@
         <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1824,13 +1827,13 @@
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1850,13 +1853,13 @@
         <v>2</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
@@ -1879,13 +1882,13 @@
         <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>17</v>
@@ -1908,13 +1911,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1937,13 +1940,13 @@
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
@@ -1966,13 +1969,13 @@
         <v>3</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1995,13 +1998,13 @@
         <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>17</v>
@@ -2024,13 +2027,13 @@
         <v>3</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>17</v>
@@ -2053,13 +2056,13 @@
         <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
@@ -2071,7 +2074,7 @@
         <v>18</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>20</v>
@@ -2082,13 +2085,13 @@
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -2108,13 +2111,13 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
@@ -2137,13 +2140,13 @@
         <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
@@ -2155,7 +2158,7 @@
         <v>18</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>20</v>
@@ -2166,13 +2169,13 @@
         <v>4</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>17</v>
@@ -2195,13 +2198,13 @@
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>17</v>
@@ -2224,13 +2227,13 @@
         <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>17</v>
@@ -2250,13 +2253,13 @@
         <v>5</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
@@ -2276,13 +2279,13 @@
         <v>5</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
@@ -2302,13 +2305,13 @@
         <v>5</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>17</v>
@@ -2328,13 +2331,13 @@
         <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>17</v>
@@ -2357,13 +2360,13 @@
         <v>5</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -2383,13 +2386,13 @@
         <v>5</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -2409,13 +2412,13 @@
         <v>5</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>17</v>
@@ -2435,13 +2438,13 @@
         <v>5</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>17</v>
@@ -2453,7 +2456,7 @@
         <v>15</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2461,13 +2464,13 @@
         <v>5</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
@@ -2487,13 +2490,13 @@
         <v>5</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
@@ -2513,25 +2516,25 @@
         <v>6</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>20</v>
@@ -2542,13 +2545,13 @@
         <v>6</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>17</v>
@@ -2557,7 +2560,7 @@
         <v>14</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>23</v>
@@ -2571,13 +2574,13 @@
         <v>6</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>17</v>
@@ -2600,13 +2603,13 @@
         <v>6</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>17</v>
@@ -2629,13 +2632,13 @@
         <v>6</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -2650,7 +2653,7 @@
         <v>23</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,13 +2661,13 @@
         <v>6</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>17</v>
@@ -2684,25 +2687,25 @@
         <v>6</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>20</v>
@@ -2713,13 +2716,13 @@
         <v>6</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>17</v>
@@ -2728,7 +2731,7 @@
         <v>14</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>23</v>
@@ -2742,13 +2745,13 @@
         <v>6</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>17</v>
@@ -2771,13 +2774,13 @@
         <v>6</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>17</v>
@@ -2800,13 +2803,13 @@
         <v>6</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>17</v>
@@ -2821,7 +2824,7 @@
         <v>23</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,13 +2832,13 @@
         <v>6</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>17</v>
@@ -2855,13 +2858,13 @@
         <v>6</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2870,7 +2873,7 @@
         <v>14</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>23</v>

</xml_diff>